<commit_message>
Import template table updated with enum values for categories
</commit_message>
<xml_diff>
--- a/storage/app/public/excel_import/import_template.xlsx
+++ b/storage/app/public/excel_import/import_template.xlsx
@@ -4,11 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Expennses" sheetId="1" r:id="rId1"/>
+    <sheet name="Categories" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="CategoriesEnum">Categories!$A$1:$A$9</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -19,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -28,6 +32,33 @@
   </si>
   <si>
     <t>Category</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Bills</t>
+  </si>
+  <si>
+    <t>Clothes and footwear</t>
+  </si>
+  <si>
+    <t>Maintenance</t>
+  </si>
+  <si>
+    <t>Education expenses</t>
+  </si>
+  <si>
+    <t>Books and other supplies</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>Medical expenses</t>
+  </si>
+  <si>
+    <t>Miscellaneous</t>
   </si>
 </sst>
 </file>
@@ -379,17 +410,17 @@
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -400,253 +431,321 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576">
+      <formula1>CategoriesEnum</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>